<commit_message>
doc: update tutorial model files
to make those compliant with the latest changes in the RAVEN model structure and GEM import/export functions
</commit_message>
<xml_diff>
--- a/tutorial/small.xlsx
+++ b/tutorial/small.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simmarc/Box Sync/3_functions/0_matlab/RAVEN/tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A533CC2-D8E0-447D-A89C-E4D2B99EA60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RXNS" sheetId="1" r:id="rId1"/>
@@ -17,20 +18,12 @@
     <sheet name="COMPS" sheetId="3" r:id="rId3"/>
     <sheet name="MODEL" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="194">
   <si>
     <t>#</t>
   </si>
@@ -578,7 +571,10 @@
     <t>cytosol</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
+    <t>boundary</t>
+  </si>
+  <si>
+    <t>TAXONOMY</t>
   </si>
   <si>
     <t>DEFAULT LOWER</t>
@@ -599,40 +595,22 @@
     <t>ORGANIZATION</t>
   </si>
   <si>
-    <t>TAXONOMY</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
-    <t>Rasmus</t>
-  </si>
-  <si>
-    <t>Agren</t>
-  </si>
-  <si>
-    <t>rasmus.agren@scilifelab.se</t>
-  </si>
-  <si>
-    <t>Chalmers University of Technology</t>
+    <t>small</t>
+  </si>
+  <si>
+    <t>Small model structure</t>
   </si>
   <si>
     <t>For use in the RAVEN workshop</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>boundary</t>
-  </si>
-  <si>
-    <t>Small model structure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,17 +675,20 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -752,9 +733,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -782,14 +763,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -817,6 +815,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -968,7 +983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -976,24 +991,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="15" width="30.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -1056,8 +1071,11 @@
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1070,8 +1088,11 @@
       <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P3" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1084,8 +1105,11 @@
       <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P4" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1098,8 +1122,11 @@
       <c r="J5" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P5" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1112,8 +1139,11 @@
       <c r="J6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P6" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1126,8 +1156,11 @@
       <c r="J7" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P7" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1140,8 +1173,11 @@
       <c r="J8" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P8" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1154,8 +1190,11 @@
       <c r="J9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P9" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1168,8 +1207,11 @@
       <c r="J10" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P10" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
@@ -1182,8 +1224,11 @@
       <c r="J11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P11" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1196,8 +1241,11 @@
       <c r="J12" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P12" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1210,8 +1258,11 @@
       <c r="J13" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P13" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1224,8 +1275,11 @@
       <c r="J14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P14" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
@@ -1238,8 +1292,11 @@
       <c r="J15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P15" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1252,8 +1309,11 @@
       <c r="J16" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P16" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
@@ -1266,8 +1326,11 @@
       <c r="J17" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P17" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
@@ -1280,8 +1343,11 @@
       <c r="J18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P18" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -1294,13 +1360,21 @@
       <c r="J19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P19" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>71</v>
       </c>
@@ -1316,8 +1390,11 @@
       <c r="J21" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P21" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
@@ -1330,8 +1407,11 @@
       <c r="J22" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P22" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1344,8 +1424,11 @@
       <c r="J23" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P23" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>81</v>
       </c>
@@ -1358,8 +1441,11 @@
       <c r="J24" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P24" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>84</v>
       </c>
@@ -1372,13 +1458,21 @@
       <c r="J25" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P25" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="P26" s="7"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>87</v>
       </c>
@@ -1393,6 +1487,9 @@
       </c>
       <c r="J27" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="P27" s="1" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +1498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1409,18 +1506,18 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1452,7 +1549,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>94</v>
       </c>
@@ -1469,7 +1566,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>97</v>
       </c>
@@ -1486,7 +1583,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>100</v>
       </c>
@@ -1503,7 +1600,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>103</v>
       </c>
@@ -1520,7 +1617,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>106</v>
       </c>
@@ -1537,7 +1634,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>109</v>
       </c>
@@ -1551,7 +1648,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>112</v>
       </c>
@@ -1565,7 +1662,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>115</v>
       </c>
@@ -1579,7 +1676,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>118</v>
       </c>
@@ -1593,7 +1690,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>121</v>
       </c>
@@ -1607,7 +1704,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>123</v>
       </c>
@@ -1621,7 +1718,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>126</v>
       </c>
@@ -1635,7 +1732,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>128</v>
       </c>
@@ -1652,7 +1749,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>132</v>
       </c>
@@ -1666,7 +1763,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>135</v>
       </c>
@@ -1680,7 +1777,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>138</v>
       </c>
@@ -1697,7 +1794,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>141</v>
       </c>
@@ -1711,7 +1808,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>144</v>
       </c>
@@ -1725,7 +1822,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>147</v>
       </c>
@@ -1742,7 +1839,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>149</v>
       </c>
@@ -1756,7 +1853,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>152</v>
       </c>
@@ -1770,7 +1867,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>155</v>
       </c>
@@ -1784,7 +1881,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>158</v>
       </c>
@@ -1798,7 +1895,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>161</v>
       </c>
@@ -1812,7 +1909,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>163</v>
       </c>
@@ -1826,7 +1923,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>165</v>
       </c>
@@ -1840,7 +1937,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>167</v>
       </c>
@@ -1857,7 +1954,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>169</v>
       </c>
@@ -1874,7 +1971,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>171</v>
       </c>
@@ -1891,7 +1988,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>173</v>
       </c>
@@ -1905,7 +2002,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>175</v>
       </c>
@@ -1928,7 +2025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1936,16 +2033,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +2059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1970,7 +2067,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1978,12 +2075,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +2089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2000,19 +2097,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2020,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>182</v>
+        <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>183</v>
@@ -2047,33 +2144,21 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="7">
-        <v>-1000</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>